<commit_message>
Version 11: added replace function for DBSheets, fixed DBMapper recordset closing + display of progress, fixed connection string setting at initialization (was set to first, not to default one)
</commit_message>
<xml_diff>
--- a/test/DBSheetsTestMSSQL.xlsx
+++ b/test/DBSheetsTestMSSQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2007F2-DB42-4B21-83A6-921BD8584E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022E4851-059E-4973-9D92-237E6E7CBCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="authors" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="LSroysched" sheetId="9" state="hidden" r:id="rId8"/>
     <sheet name="roysched" sheetId="8" r:id="rId9"/>
     <sheet name="LStitleauthor" sheetId="11" state="hidden" r:id="rId10"/>
-    <sheet name="b368a3dd6ec44ad6b0ff6e1b5d9d47c" sheetId="15" state="hidden" r:id="rId11"/>
+    <sheet name="LSsales" sheetId="15" state="hidden" r:id="rId11"/>
     <sheet name="sales" sheetId="14" r:id="rId12"/>
     <sheet name="titleauthor" sheetId="10" r:id="rId13"/>
     <sheet name="LStitles" sheetId="13" state="hidden" r:id="rId14"/>
@@ -38,7 +38,7 @@
     <definedName name="DBFsource2517e42db6d745919f56c8af78e36649" hidden="1">LStitles!$B$1</definedName>
     <definedName name="DBFsource2667b199dcf74132bf39cc670625fd17" hidden="1">titleauthor!$A$1</definedName>
     <definedName name="DBFsource6d3053372ec04b5685ae1ae8b1ec3eb4" hidden="1">roysched!$A$1</definedName>
-    <definedName name="DBFsource9444f24f32684e17951052ebf4950abb" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$C$1</definedName>
+    <definedName name="DBFsource9444f24f32684e17951052ebf4950abb" hidden="1">LSsales!$C$1</definedName>
     <definedName name="DBFsource992c0b939c834927b5b4be12e7c5f3bc" hidden="1">#REF!</definedName>
     <definedName name="DBFsource9dcfa89545974284a4e8215f57a7dc41" hidden="1">discounts!$A$1</definedName>
     <definedName name="DBFsourceafaeef3da22240e7856064ff43f8d6d8" hidden="1">publishers!$A$1</definedName>
@@ -48,33 +48,33 @@
     <definedName name="DBFsourced71aa659a0864d838c2b664cc128979b" hidden="1">LSroysched!$A$1</definedName>
     <definedName name="DBFsourced7f34f9f057d494fa071dbec688c6080" hidden="1">authors!$A$1</definedName>
     <definedName name="DBFsourcedc77197d6da141ce80332f033e31f791" hidden="1">titles!$A$1</definedName>
-    <definedName name="DBFsourcedf6827daae9247819721166790c967f4" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$A$1</definedName>
+    <definedName name="DBFsourcedf6827daae9247819721166790c967f4" hidden="1">LSsales!$A$1</definedName>
     <definedName name="DBFsourcee6eb8d79946a4d6f8ace0a53c821007e" hidden="1">sales!$A$1</definedName>
     <definedName name="DBFsourcef29a24267b8d48e484d50125828ea001" hidden="1">LStitleauthor!$A$1</definedName>
     <definedName name="DBFsourcef4ff6127b9e24ce29b99ad13e11762a6" hidden="1">LSemployee!$A$1</definedName>
-    <definedName name="DBFtarget008b1f5c6c9e4da4bb8c477f6a375b1a" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$A$2:$B$7</definedName>
+    <definedName name="DBFtarget008b1f5c6c9e4da4bb8c477f6a375b1a" hidden="1">LSsales!$A$2:$B$7</definedName>
     <definedName name="DBFtarget048386b80dec4e9d87cf9513847ac5db" hidden="1">#REF!</definedName>
-    <definedName name="DBFtarget16088adc084140e59ac953b64c5809af" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$C$2:$D$18</definedName>
+    <definedName name="DBFtarget16088adc084140e59ac953b64c5809af" hidden="1">LSsales!$C$2:$D$18</definedName>
     <definedName name="DBFtarget2517e42db6d745919f56c8af78e36649" hidden="1">LStitles!$B$2:$C$9</definedName>
     <definedName name="DBFtarget2667b199dcf74132bf39cc670625fd17" hidden="1">titleauthor!$B$1:$G$25</definedName>
     <definedName name="DBFtarget6d3053372ec04b5685ae1ae8b1ec3eb4" hidden="1">roysched!$B$1:$F$87</definedName>
-    <definedName name="DBFtarget9444f24f32684e17951052ebf4950abb" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$C$2:$D$18</definedName>
+    <definedName name="DBFtarget9444f24f32684e17951052ebf4950abb" hidden="1">LSsales!$C$2:$D$18</definedName>
     <definedName name="DBFtarget992c0b939c834927b5b4be12e7c5f3bc" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget9dcfa89545974284a4e8215f57a7dc41" hidden="1">discounts!$B$1:$G$4</definedName>
     <definedName name="DBFtargetafaeef3da22240e7856064ff43f8d6d8" hidden="1">publishers!$B$1:$F$9</definedName>
-    <definedName name="DBFtargetb648a6b572ea4b258d6eddefa1f1a1a2" hidden="1">employee!$B$1:$J$44</definedName>
+    <definedName name="DBFtargetb648a6b572ea4b258d6eddefa1f1a1a2" hidden="1">employee!$B$1:$J$48</definedName>
     <definedName name="DBFtargetba58cf4be2a54e63af8d36a10a2307ca" hidden="1">jobs!$B$1:$E$15</definedName>
     <definedName name="DBFtargetbbf44909fbc248689a82885fda31d908" hidden="1">LStitles!$B$2:$C$9</definedName>
-    <definedName name="DBFtargetd71aa659a0864d838c2b664cc128979b" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$C$2:$D$18</definedName>
+    <definedName name="DBFtargetd71aa659a0864d838c2b664cc128979b" hidden="1">LSsales!$C$2:$D$18</definedName>
     <definedName name="DBFtargetd7f34f9f057d494fa071dbec688c6080" hidden="1">authors!$B$1:$J$24</definedName>
     <definedName name="DBFtargetdc77197d6da141ce80332f033e31f791" hidden="1">titles!$B$1:$L$18</definedName>
-    <definedName name="DBFtargetdf6827daae9247819721166790c967f4" hidden="1">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$A$2:$B$7</definedName>
+    <definedName name="DBFtargetdf6827daae9247819721166790c967f4" hidden="1">LSsales!$A$2:$B$7</definedName>
     <definedName name="DBFtargete6eb8d79946a4d6f8ace0a53c821007e" hidden="1">sales!$B$1:$I$22</definedName>
     <definedName name="DBFtargetf29a24267b8d48e484d50125828ea001" hidden="1">LStitleauthor!$A$2:$B$24</definedName>
     <definedName name="DBFtargetf4ff6127b9e24ce29b99ad13e11762a6" hidden="1">LSemployee!$A$2:$B$15</definedName>
     <definedName name="DBMapperauthors">authors!$B$1:$J$24</definedName>
     <definedName name="DBMapperdiscounts">discounts!$B$1:$G$4</definedName>
-    <definedName name="DBMapperemployee">employee!$B$1:$J$44</definedName>
+    <definedName name="DBMapperemployee">employee!$B$1:$J$48</definedName>
     <definedName name="DBMapperjobs">jobs!$B$1:$E$15</definedName>
     <definedName name="DBMapperpublishers">publishers!$B$1:$F$9</definedName>
     <definedName name="DBMapperpubs.dbo.sales">sales!$B$1:$I$22</definedName>
@@ -83,7 +83,7 @@
     <definedName name="DBMappertitles">titles!$B$1:$L$18</definedName>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">authors!$B$1:$J$24</definedName>
     <definedName name="ExterneDaten_1" localSheetId="2" hidden="1">discounts!$B$1:$F$4</definedName>
-    <definedName name="ExterneDaten_1" localSheetId="4" hidden="1">employee!$B$1:$H$44</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="4" hidden="1">employee!$B$1:$H$48</definedName>
     <definedName name="ExterneDaten_1" localSheetId="5" hidden="1">jobs!$B$1:$E$15</definedName>
     <definedName name="ExterneDaten_1" localSheetId="6" hidden="1">publishers!$B$1:$F$9</definedName>
     <definedName name="ExterneDaten_1" localSheetId="8" hidden="1">roysched!$B$1:$E$87</definedName>
@@ -92,8 +92,8 @@
     <definedName name="ExterneDaten_1" localSheetId="14" hidden="1">titles!$B$1:$K$18</definedName>
     <definedName name="job_idLookup">LSemployee!$A$2:$B$15</definedName>
     <definedName name="pub_idLookup">LStitles!$B$2:$C$9</definedName>
-    <definedName name="stor_idLookup">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$A$2:$B$7</definedName>
-    <definedName name="title_idLookup">b368a3dd6ec44ad6b0ff6e1b5d9d47c!$C$2:$D$18</definedName>
+    <definedName name="stor_idLookup">LSsales!$A$2:$B$7</definedName>
+    <definedName name="title_idLookup">LSsales!$C$2:$D$18</definedName>
     <definedName name="typeLookup">LStitles!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="543">
   <si>
     <t xml:space="preserve">SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000D_
 FROM pubs.dbo.authors T1 _x000D_
@@ -1381,9 +1381,6 @@
     <t>PS2106</t>
   </si>
   <si>
-    <t>PC9999</t>
-  </si>
-  <si>
     <t>Onions, Leeks, and Garlic: Cooking Secrets of the Mediterranean/Binnet &amp; Hardley</t>
   </si>
   <si>
@@ -1556,9 +1553,6 @@
     <t>Life Without Fear</t>
   </si>
   <si>
-    <t>Net Etiquette</t>
-  </si>
-  <si>
     <t>Onions, Leeks, and Garlic: Cooking Secrets of the Mediterranean</t>
   </si>
   <si>
@@ -1688,16 +1682,10 @@
     <t>Detailed instructions on how to make authentic Japanese sushi in your spare time.</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>Chief Executive Officer</t>
   </si>
   <si>
     <t>309 63rd St. #411</t>
-  </si>
-  <si>
-    <t>Mnchen</t>
   </si>
   <si>
     <t xml:space="preserve">SELECT T2.stor_name AS stor_idLU, T1.ord_num, T1.ord_date, T1.qty, T1.payterms, T7.title AS title_idLU_x000D_
@@ -1780,6 +1768,42 @@
   </si>
   <si>
     <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>PMA42628M</t>
+  </si>
+  <si>
+    <t>DZT39435M</t>
+  </si>
+  <si>
+    <t>iouiz</t>
+  </si>
+  <si>
+    <t>iuziuz</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>DZT39436F</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>rtzrfh</t>
+  </si>
+  <si>
+    <t>DBT39435F</t>
+  </si>
+  <si>
+    <t>swer</t>
+  </si>
+  <si>
+    <t>München</t>
   </si>
 </sst>
 </file>
@@ -3316,7 +3340,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle_ExterneDaten_14" displayName="Tabelle_ExterneDaten_14" ref="B1:J44" tableType="queryTable" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle_ExterneDaten_14" displayName="Tabelle_ExterneDaten_14" ref="B1:J48" tableType="queryTable" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <tableColumns count="9">
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="59"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="58"/>
@@ -3698,6 +3722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3710,7 +3735,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
@@ -3837,7 +3862,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
@@ -4472,6 +4497,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Tabelle10"/>
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4484,19 +4510,19 @@
         <v>Env:MSSQL, (last result:)Retrieved 23 records from: SELECT T1.au_lname + ' ' + T1.au_fname au_id,T1.au_id FROM pubs.dbo.authors T1 ORDER BY T1.au_lname</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C1" t="str">
         <f>_xll.DBListFetch(D1,"",title_idLookup)</f>
         <v>Env:MSSQL, (last result:)Retrieved 17 records from: SELECT title,title_id FROM pubs.dbo.titles ORDER BY title</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
@@ -4504,7 +4530,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
@@ -4512,7 +4538,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -4520,7 +4546,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B5" t="s">
         <v>109</v>
@@ -4528,7 +4554,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B6" t="s">
         <v>101</v>
@@ -4536,7 +4562,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
@@ -4544,7 +4570,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -4552,7 +4578,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
@@ -4560,7 +4586,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
@@ -4568,7 +4594,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B11" t="s">
         <v>141</v>
@@ -4576,7 +4602,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B12" t="s">
         <v>128</v>
@@ -4584,7 +4610,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B13" t="s">
         <v>71</v>
@@ -4592,7 +4618,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
@@ -4600,7 +4626,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B15" t="s">
         <v>144</v>
@@ -4608,7 +4634,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
@@ -4616,7 +4642,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B17" t="s">
         <v>133</v>
@@ -4624,7 +4650,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B18" t="s">
         <v>159</v>
@@ -4632,7 +4658,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B19" t="s">
         <v>151</v>
@@ -4640,7 +4666,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -4648,7 +4674,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
@@ -4656,7 +4682,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B22" t="s">
         <v>117</v>
@@ -4664,7 +4690,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -4672,7 +4698,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B24" t="s">
         <v>94</v>
@@ -4685,9 +4711,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD134784-0593-4A30-A7DE-A828677A326F}">
+  <sheetPr codeName="Tabelle11"/>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4704,7 +4733,7 @@
         <v>Env:MSSQL, (last result:)Retrieved 17 records from: SELECT title,title_id FROM pubs.dbo.titles ORDER BY title</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4715,10 +4744,10 @@
         <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>529</v>
       </c>
       <c r="D2" t="s">
-        <v>392</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4729,10 +4758,10 @@
         <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4743,10 +4772,10 @@
         <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4757,10 +4786,10 @@
         <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4771,10 +4800,10 @@
         <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,98 +4814,98 @@
         <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -4886,13 +4915,14 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE1A2A5-8455-4488-BB08-CAF73C694F74}">
+  <sheetPr codeName="Tabelle12"/>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,36 +4949,36 @@
         <v>176</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>183</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D2" s="4">
         <v>34591</v>
@@ -4957,10 +4987,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -4976,7 +5006,7 @@
         <v>169</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D3" s="4">
         <v>34590</v>
@@ -4985,10 +5015,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H3" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5004,7 +5034,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D4" s="4">
         <v>34591</v>
@@ -5013,10 +5043,10 @@
         <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5032,7 +5062,7 @@
         <v>163</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D5" s="4">
         <v>34590</v>
@@ -5041,10 +5071,10 @@
         <v>75</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H5" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5060,7 +5090,7 @@
         <v>173</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D6" s="4">
         <v>34591</v>
@@ -5069,10 +5099,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H6" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5088,7 +5118,7 @@
         <v>173</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D7" s="4">
         <v>33770</v>
@@ -5097,10 +5127,10 @@
         <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H7" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5116,7 +5146,7 @@
         <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D8" s="4">
         <v>33770</v>
@@ -5125,10 +5155,10 @@
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H8" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5144,7 +5174,7 @@
         <v>173</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D9" s="4">
         <v>33770</v>
@@ -5153,10 +5183,10 @@
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H9" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5172,7 +5202,7 @@
         <v>167</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D10" s="4">
         <v>34591</v>
@@ -5181,10 +5211,10 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H10" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5200,7 +5230,7 @@
         <v>167</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D11" s="4">
         <v>34591</v>
@@ -5209,10 +5239,10 @@
         <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H11" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5228,7 +5258,7 @@
         <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D12" s="4">
         <v>34118</v>
@@ -5237,10 +5267,10 @@
         <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H12" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5256,7 +5286,7 @@
         <v>167</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D13" s="4">
         <v>34118</v>
@@ -5265,10 +5295,10 @@
         <v>25</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5284,7 +5314,7 @@
         <v>167</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D14" s="4">
         <v>34118</v>
@@ -5293,10 +5323,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H14" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5312,7 +5342,7 @@
         <v>167</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D15" s="4">
         <v>34118</v>
@@ -5321,10 +5351,10 @@
         <v>25</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H15" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5340,7 +5370,7 @@
         <v>171</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D16" s="4">
         <v>34270</v>
@@ -5349,10 +5379,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H16" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5368,7 +5398,7 @@
         <v>171</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D17" s="4">
         <v>34315</v>
@@ -5377,10 +5407,10 @@
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H17" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5396,7 +5426,7 @@
         <v>171</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D18" s="4">
         <v>34021</v>
@@ -5405,10 +5435,10 @@
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H18" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5424,7 +5454,7 @@
         <v>165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D19" s="4">
         <v>34591</v>
@@ -5433,10 +5463,10 @@
         <v>10</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H19" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5452,7 +5482,7 @@
         <v>165</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D20" s="4">
         <v>33770</v>
@@ -5461,10 +5491,10 @@
         <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H20" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5480,7 +5510,7 @@
         <v>165</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D21" s="4">
         <v>34039</v>
@@ -5489,10 +5519,10 @@
         <v>25</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H21" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5508,7 +5538,7 @@
         <v>165</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D22" s="4">
         <v>34111</v>
@@ -5517,10 +5547,10 @@
         <v>30</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H22" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_110[[#This Row],[stor_idLU]],stor_idLookup,2,FALSE),"")</f>
@@ -5549,6 +5579,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Tabelle13"/>
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -5576,33 +5607,33 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -5621,10 +5652,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -5643,10 +5674,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -5665,10 +5696,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -5687,10 +5718,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -5709,10 +5740,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -5731,10 +5762,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -5753,10 +5784,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -5775,10 +5806,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -5797,10 +5828,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -5819,10 +5850,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -5841,10 +5872,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -5863,10 +5894,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -5885,10 +5916,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -5907,10 +5938,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -5929,10 +5960,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -5951,10 +5982,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -5973,10 +6004,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -5995,10 +6026,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -6017,10 +6048,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
@@ -6039,10 +6070,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -6061,10 +6092,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
@@ -6083,10 +6114,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -6105,10 +6136,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -6144,6 +6175,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Tabelle14"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6156,12 +6188,12 @@
         <v>Env:MSSQL, (last result:)Retrieved 8 records from: SELECT pub_name,pub_id FROM pubs.dbo.publishers ORDER BY pub_name</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B2" t="s">
         <v>214</v>
@@ -6172,7 +6204,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B3" t="s">
         <v>212</v>
@@ -6183,7 +6215,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B4" t="s">
         <v>210</v>
@@ -6194,7 +6226,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B5" t="s">
         <v>208</v>
@@ -6205,7 +6237,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
@@ -6245,10 +6277,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Tabelle15"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6276,34 +6309,34 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>222</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>488</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>367</v>
@@ -6311,16 +6344,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>214</v>
@@ -6338,7 +6371,7 @@
         <v>4095</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K2" s="4">
         <v>33401</v>
@@ -6353,10 +6386,10 @@
         <v>396</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>214</v>
@@ -6374,7 +6407,7 @@
         <v>3876</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K3" s="4">
         <v>33398</v>
@@ -6386,13 +6419,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>204</v>
@@ -6410,7 +6443,7 @@
         <v>18722</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K4" s="4">
         <v>33419</v>
@@ -6422,13 +6455,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>214</v>
@@ -6446,7 +6479,7 @@
         <v>4095</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K5" s="4">
         <v>33411</v>
@@ -6458,13 +6491,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>212</v>
@@ -6482,7 +6515,7 @@
         <v>2032</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K6" s="4">
         <v>33398</v>
@@ -6494,13 +6527,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>212</v>
@@ -6518,7 +6551,7 @@
         <v>22246</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K7" s="4">
         <v>33407</v>
@@ -6533,10 +6566,10 @@
         <v>392</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>214</v>
@@ -6554,7 +6587,7 @@
         <v>8780</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="K8" s="4">
         <v>33419</v>
@@ -6566,13 +6599,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>214</v>
@@ -6590,7 +6623,7 @@
         <v>4095</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="K9" s="4">
         <v>34497</v>
@@ -6605,10 +6638,10 @@
         <v>394</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>212</v>
@@ -6626,7 +6659,7 @@
         <v>375</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K10" s="4">
         <v>33532</v>
@@ -6641,10 +6674,10 @@
         <v>402</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>204</v>
@@ -6662,7 +6695,7 @@
         <v>2045</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="K11" s="4">
         <v>33404</v>
@@ -6677,10 +6710,10 @@
         <v>404</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>204</v>
@@ -6698,7 +6731,7 @@
         <v>111</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K12" s="4">
         <v>33516</v>
@@ -6710,13 +6743,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>204</v>
@@ -6734,7 +6767,7 @@
         <v>4072</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K13" s="4">
         <v>33401</v>
@@ -6749,10 +6782,10 @@
         <v>398</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>204</v>
@@ -6770,7 +6803,7 @@
         <v>3336</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K14" s="4">
         <v>33401</v>
@@ -6782,13 +6815,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>212</v>
@@ -6806,7 +6839,7 @@
         <v>375</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K15" s="4">
         <v>33532</v>
@@ -6818,13 +6851,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>208</v>
@@ -6834,7 +6867,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K16" s="4">
         <v>33532</v>
@@ -6849,10 +6882,10 @@
         <v>400</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>212</v>
@@ -6870,7 +6903,7 @@
         <v>15096</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="K17" s="4">
         <v>33532</v>
@@ -6882,13 +6915,13 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>212</v>
@@ -6906,7 +6939,7 @@
         <v>4095</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K18" s="4">
         <v>33401</v>
@@ -6934,6 +6967,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6956,6 +6990,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7069,6 +7104,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7181,7 +7217,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -7210,7 +7246,8 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J44"/>
+  <sheetPr codeName="Tabelle5"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -7284,17 +7321,17 @@
         <v>226</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G2" s="3">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>208</v>
       </c>
       <c r="I2" s="3">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7303,91 +7340,91 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>228</v>
+        <v>531</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G3" s="2">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I3" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G4" s="2">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I4" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J4" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>505</v>
+        <v>234</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G5" s="2">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I5" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J5" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7396,29 +7433,27 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>241</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G6" s="2">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I6" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7427,58 +7462,58 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>240</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G7" s="2">
-        <v>227</v>
+        <v>120</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="I7" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J7" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9952</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>248</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G8" s="2">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>200</v>
       </c>
       <c r="I8" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7487,29 +7522,29 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G9" s="2">
-        <v>87</v>
+        <v>215</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>200</v>
       </c>
       <c r="I9" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J9" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7518,91 +7553,91 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>251</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G10" s="2">
-        <v>200</v>
+        <v>87</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="I10" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J10" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9952</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>257</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G11" s="2">
-        <v>77</v>
+        <v>200</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="I11" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J11" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9952</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G12" s="2">
-        <v>159</v>
+        <v>77</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>212</v>
       </c>
       <c r="I12" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J12" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -7611,25 +7646,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>188</v>
       </c>
       <c r="G13" s="2">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I13" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -7637,557 +7672,559 @@
       </c>
       <c r="J13" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G14" s="2">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I14" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J14" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G15" s="2">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I15" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J15" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>276</v>
+        <v>532</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>266</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>278</v>
+        <v>534</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G16" s="2">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I16" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J16" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G17" s="2">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I17" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J17" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G18" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I18" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J18" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G19" s="2">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I19" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J19" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9901</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>241</v>
+        <v>285</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G20" s="2">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I20" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J20" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>288</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G21" s="2">
-        <v>77</v>
+        <v>172</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="I21" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J21" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9901</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G22" s="2">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I22" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J22" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>302</v>
+        <v>535</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G23" s="2">
         <v>77</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I23" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J23" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>306</v>
+        <v>225</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G24" s="2">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I24" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J24" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="E25" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G25" s="2">
-        <v>150</v>
+        <v>77</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I25" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J25" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>227</v>
+        <v>306</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G26" s="2">
-        <v>198</v>
+        <v>150</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I26" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J26" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1622</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>225</v>
+        <v>535</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G27" s="2">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I27" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J27" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G28" s="2">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="I28" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J28" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>321</v>
+        <v>225</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G29" s="2">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I29" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J29" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>324</v>
+        <v>536</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G30" s="2">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I30" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J30" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0736</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>230</v>
+        <v>321</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G31" s="2">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I31" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J31" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -8196,85 +8233,87 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D32" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="E32" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G32" s="2">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I32" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J32" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>292</v>
+        <v>327</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G33" s="2">
-        <v>246</v>
+        <v>125</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="I33" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J33" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1756</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>336</v>
+        <v>535</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>188</v>
+        <v>331</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>189</v>
       </c>
       <c r="G34" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I34" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -8282,185 +8321,187 @@
       </c>
       <c r="J34" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>292</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>274</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G35" s="2">
-        <v>77</v>
+        <v>246</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="I35" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J35" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0877</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>343</v>
+        <v>188</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G36" s="2">
-        <v>192</v>
+        <v>100</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I36" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J36" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>338</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>535</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G37" s="2">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I37" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J37" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>9999</v>
+        <v>0877</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>254</v>
+        <v>342</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G38" s="2">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I38" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J38" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>281</v>
+        <v>535</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G39" s="2">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I39" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J39" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>1389</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>353</v>
+        <v>537</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>225</v>
-      </c>
+        <v>538</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>45</v>
+        <v>539</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G40" s="2">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>214</v>
       </c>
       <c r="I40" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J40" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -8469,29 +8510,29 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G41" s="2">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>204</v>
       </c>
       <c r="I41" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J41" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
@@ -8500,56 +8541,56 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G42" s="2">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I42" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J42" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>114</v>
+        <v>354</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>362</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>199</v>
       </c>
       <c r="G43" s="2">
-        <v>170</v>
+        <v>78</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I43" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
@@ -8557,46 +8598,170 @@
       </c>
       <c r="J43" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
-        <v>0736</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G44" s="2">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I44" s="2">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J44" s="2" t="str">
         <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
+        <v>0736</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G45" s="2">
+        <v>165</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I45" s="2">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
+        <v>10</v>
+      </c>
+      <c r="J45" s="2" t="str">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
+        <v>0736</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G46" s="2">
+        <v>77</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I46" s="2">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
+        <v>13</v>
+      </c>
+      <c r="J46" s="2" t="str">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
+        <v>0877</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G47" s="2">
+        <v>170</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I47" s="2">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
+        <v>9</v>
+      </c>
+      <c r="J47" s="2" t="str">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
+        <v>0736</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G48" s="2">
+        <v>77</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I48" s="2">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[job_idLU]],job_idLookup,2,FALSE),"")</f>
+        <v>11</v>
+      </c>
+      <c r="J48" s="2" t="str">
+        <f>IF(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_14[[#This Row],[pub_idLU]],pub_idLookup,2,FALSE),"")</f>
         <v>0877</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F48" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>OFFSET(job_idLookup,0,0,,1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H44" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H48" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>OFFSET(pub_idLookup,0,0,,1)</formula1>
     </dataValidation>
   </dataValidations>
@@ -8609,6 +8774,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8667,7 +8833,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -8854,6 +9020,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8990,7 +9157,7 @@
         <v>208</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>508</v>
+        <v>542</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -9039,6 +9206,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9061,6 +9229,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Tabelle9"/>
   <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9087,19 +9256,19 @@
 </v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9107,7 +9276,7 @@
         <v>390</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -9129,7 +9298,7 @@
         <v xml:space="preserve">WHERE T1.lorange &gt;  and T1.hirange &lt; </v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C3" s="2">
         <v>5001</v>
@@ -9237,7 +9406,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -9255,7 +9424,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C10" s="2">
         <v>1001</v>
@@ -9273,7 +9442,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C11" s="2">
         <v>3001</v>
@@ -9291,7 +9460,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C12" s="2">
         <v>5001</v>
@@ -9309,7 +9478,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C13" s="2">
         <v>7001</v>
@@ -9327,7 +9496,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C14" s="2">
         <v>10001</v>
@@ -9345,7 +9514,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C15" s="2">
         <v>12001</v>
@@ -9363,7 +9532,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C16" s="2">
         <v>14001</v>
@@ -9525,7 +9694,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -9543,7 +9712,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C26" s="2">
         <v>1001</v>
@@ -9561,7 +9730,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C27" s="2">
         <v>2001</v>
@@ -9579,7 +9748,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C28" s="2">
         <v>4001</v>
@@ -9597,7 +9766,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C29" s="2">
         <v>6001</v>
@@ -9615,7 +9784,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C30" s="2">
         <v>8001</v>
@@ -9633,7 +9802,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C31" s="2">
         <v>10001</v>
@@ -9651,7 +9820,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C32" s="2">
         <v>12001</v>
@@ -9669,7 +9838,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -9687,7 +9856,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C34" s="2">
         <v>2001</v>
@@ -9705,7 +9874,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C35" s="2">
         <v>4001</v>
@@ -9723,7 +9892,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C36" s="2">
         <v>6001</v>
@@ -9741,7 +9910,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C37" s="2">
         <v>8001</v>
@@ -9759,7 +9928,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C38" s="2">
         <v>10001</v>
@@ -9777,7 +9946,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C39" s="2">
         <v>12001</v>
@@ -9795,7 +9964,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C40" s="2">
         <v>14001</v>
@@ -9813,7 +9982,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
@@ -9831,7 +10000,7 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C42" s="2">
         <v>5001</v>
@@ -9849,7 +10018,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C43" s="2">
         <v>10001</v>
@@ -9867,7 +10036,7 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C44" s="2">
         <v>15001</v>
@@ -9921,7 +10090,7 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -9939,7 +10108,7 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C48" s="2">
         <v>5001</v>
@@ -9957,7 +10126,7 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C49" s="2">
         <v>10001</v>
@@ -9975,7 +10144,7 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C50" s="2">
         <v>15001</v>
@@ -10137,7 +10306,7 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -10155,7 +10324,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C60" s="2">
         <v>2001</v>
@@ -10173,7 +10342,7 @@
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C61" s="2">
         <v>4001</v>
@@ -10191,7 +10360,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C62" s="2">
         <v>8001</v>
@@ -10209,7 +10378,7 @@
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C63" s="2">
         <v>12001</v>
@@ -10227,7 +10396,7 @@
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C64" s="2">
         <v>20001</v>
@@ -10245,7 +10414,7 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -10263,7 +10432,7 @@
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C66" s="2">
         <v>5001</v>
@@ -10281,7 +10450,7 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C67" s="2">
         <v>15001</v>
@@ -10425,7 +10594,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -10443,7 +10612,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C76" s="2">
         <v>5001</v>
@@ -10461,7 +10630,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C77" s="2">
         <v>10001</v>
@@ -10479,7 +10648,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C78" s="2">
         <v>15001</v>
@@ -10497,7 +10666,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C79" s="2">
         <v>20001</v>
@@ -10515,7 +10684,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C80" s="2">
         <v>25001</v>
@@ -10533,7 +10702,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C81" s="2">
         <v>30001</v>
@@ -10551,7 +10720,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C82" s="2">
         <v>35001</v>

</xml_diff>

<commit_message>
started change of DBModifier to ADO.NET fixed change function (returns full string now instead of empty) DBModifier message on saving workbook unified with askBeforeExecute message (and refactored)
</commit_message>
<xml_diff>
--- a/test/DBSheetsTestMSSQL.xlsx
+++ b/test/DBSheetsTestMSSQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022E4851-059E-4973-9D92-237E6E7CBCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBC25D6-C512-4696-92CF-7A21F22F6C92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5910" yWindow="1725" windowWidth="22095" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="authors" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <definedName name="DBFtarget048386b80dec4e9d87cf9513847ac5db" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget16088adc084140e59ac953b64c5809af" hidden="1">LSsales!$C$2:$D$18</definedName>
     <definedName name="DBFtarget2517e42db6d745919f56c8af78e36649" hidden="1">LStitles!$B$2:$C$9</definedName>
-    <definedName name="DBFtarget2667b199dcf74132bf39cc670625fd17" hidden="1">titleauthor!$B$1:$G$25</definedName>
+    <definedName name="DBFtarget2667b199dcf74132bf39cc670625fd17" hidden="1">titleauthor!$B$1:$G$26</definedName>
     <definedName name="DBFtarget6d3053372ec04b5685ae1ae8b1ec3eb4" hidden="1">roysched!$B$1:$F$87</definedName>
     <definedName name="DBFtarget9444f24f32684e17951052ebf4950abb" hidden="1">LSsales!$C$2:$D$18</definedName>
     <definedName name="DBFtarget992c0b939c834927b5b4be12e7c5f3bc" hidden="1">#REF!</definedName>
@@ -79,7 +79,7 @@
     <definedName name="DBMapperpublishers">publishers!$B$1:$F$9</definedName>
     <definedName name="DBMapperpubs.dbo.sales">sales!$B$1:$I$22</definedName>
     <definedName name="DBMapperroysched">roysched!$B$1:$F$87</definedName>
-    <definedName name="DBMappertitleauthor">titleauthor!$B$1:$G$25</definedName>
+    <definedName name="DBMappertitleauthor">titleauthor!$B$1:$G$26</definedName>
     <definedName name="DBMappertitles">titles!$B$1:$L$18</definedName>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">authors!$B$1:$J$24</definedName>
     <definedName name="ExterneDaten_1" localSheetId="2" hidden="1">discounts!$B$1:$F$4</definedName>
@@ -88,7 +88,7 @@
     <definedName name="ExterneDaten_1" localSheetId="6" hidden="1">publishers!$B$1:$F$9</definedName>
     <definedName name="ExterneDaten_1" localSheetId="8" hidden="1">roysched!$B$1:$E$87</definedName>
     <definedName name="ExterneDaten_1" localSheetId="11" hidden="1">sales!$B$1:$G$22</definedName>
-    <definedName name="ExterneDaten_1" localSheetId="12" hidden="1">titleauthor!$B$1:$E$25</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="12" hidden="1">titleauthor!$B$1:$E$26</definedName>
     <definedName name="ExterneDaten_1" localSheetId="14" hidden="1">titles!$B$1:$K$18</definedName>
     <definedName name="job_idLookup">LSemployee!$A$2:$B$15</definedName>
     <definedName name="pub_idLookup">LStitles!$B$2:$C$9</definedName>
@@ -116,37 +116,37 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Verbindung" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000d__x000a_FROM pubs.dbo.authors T1 _x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000d__x000a_FROM pubs.dbo.authors T1 _x000d__x000a_"/>
   </connection>
   <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Verbindung1" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.discounttype, T3.stor_name AS stor_idLU, T1.lowqty, T1.highqty, T1.discount_x000d__x000a_FROM pubs.dbo.discounts T1 LEFT JOIN _x000d__x000a_pubs.dbo.stores T3 ON T1.stor_id = T3.stor_id_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.discounttype, T3.stor_name AS stor_idLU, T1.lowqty, T1.highqty, T1.discount_x000d__x000a_FROM pubs.dbo.discounts T1 LEFT JOIN _x000d__x000a_pubs.dbo.stores T3 ON T1.stor_id = T3.stor_id_x000d__x000a_"/>
   </connection>
   <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" keepAlive="1" name="Verbindung2" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.emp_id, T1.fname, T1.minit, T1.lname, T6.job_desc AS job_idLU, T1.job_lvl, T8.pub_name AS pub_idLU_x000d__x000a_FROM pubs.dbo.employee T1 INNER JOIN _x000d__x000a_pubs.dbo.jobs T6 ON T1.job_id = T6.job_id INNER JOIN _x000d__x000a_pubs.dbo.publishers T8 ON T1.pub_id = T8.pub_id_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.emp_id, T1.fname, T1.minit, T1.lname, T6.job_desc AS job_idLU, T1.job_lvl, T8.pub_name AS pub_idLU_x000d__x000a_FROM pubs.dbo.employee T1 INNER JOIN _x000d__x000a_pubs.dbo.jobs T6 ON T1.job_id = T6.job_id INNER JOIN _x000d__x000a_pubs.dbo.publishers T8 ON T1.pub_id = T8.pub_id_x000d__x000a_"/>
   </connection>
   <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" keepAlive="1" name="Verbindung3" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.job_id, T1.job_desc, T1.min_lvl, T1.max_lvl_x000d__x000a_FROM pubs.dbo.jobs T1_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.job_id, T1.job_desc, T1.min_lvl, T1.max_lvl_x000d__x000a_FROM pubs.dbo.jobs T1_x000d__x000a_"/>
   </connection>
   <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" keepAlive="1" name="Verbindung4" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.pub_id, T1.pub_name, T1.city, T1.state, T1.country_x000d__x000a_FROM pubs.dbo.publishers T1_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.pub_id, T1.pub_name, T1.city, T1.state, T1.country_x000d__x000a_FROM pubs.dbo.publishers T1_x000d__x000a_"/>
   </connection>
   <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" keepAlive="1" name="Verbindung5" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T2.title+'/'+p.pub_name AS title_idLU, T1.lorange, T1.hirange, T1.royalty_x000d__x000a_FROM pubs.dbo.roysched T1 INNER JOIN _x000d__x000a_pubs.dbo.titles T2 ON T1.title_id = T2.title_id LEFT JOIN _x000d__x000a_pubs.dbo.publishers p ON T2.pub_id = p.pub_id_x000d__x000a__x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T2.title+'/'+p.pub_name AS title_idLU, T1.lorange, T1.hirange, T1.royalty_x000d__x000a_FROM pubs.dbo.roysched T1 INNER JOIN _x000d__x000a_pubs.dbo.titles T2 ON T1.title_id = T2.title_id LEFT JOIN _x000d__x000a_pubs.dbo.publishers p ON T2.pub_id = p.pub_id_x000d__x000a__x000d__x000a_"/>
   </connection>
   <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" keepAlive="1" name="Verbindung6" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT isnull(T2.au_lname + ' ' + T2.au_fname, T1.au_id) au_idLU, T3.title AS title_idLU, T1.au_ord, T1.royaltyper_x000d__x000a_FROM pubs.dbo.titleauthor T1 LEFT JOIN _x000d__x000a_pubs.dbo.authors T2 ON T1.au_id = T2.au_id LEFT JOIN _x000d__x000a_pubs.dbo.titles T3 ON T1.title_id = T3.title_id_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT isnull(T2.au_lname + ' ' + T2.au_fname, T1.au_id) au_idLU, T3.title AS title_idLU, T1.au_ord, T1.royaltyper_x000d__x000a_FROM pubs.dbo.titleauthor T1 LEFT JOIN _x000d__x000a_pubs.dbo.authors T2 ON T1.au_id = T2.au_id LEFT JOIN _x000d__x000a_pubs.dbo.titles T3 ON T1.title_id = T3.title_id_x000d__x000a_"/>
   </connection>
   <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" keepAlive="1" name="Verbindung7" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T1.title_id, T1.title, T1.type, T5.pub_name AS pub_idLU, T1.price, T1.advance, T1.royalty, T1.ytd_sales, T1.notes, T1.pubdate_x000d__x000a_FROM pubs.dbo.titles T1 LEFT JOIN _x000d__x000a_pubs.dbo.publishers T5 ON T1.pub_id = T5.pub_id_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T1.title_id, T1.title, T1.type, T5.pub_name AS pub_idLU, T1.price, T1.advance, T1.royalty, T1.ytd_sales, T1.notes, T1.pubdate_x000d__x000a_FROM pubs.dbo.titles T1 LEFT JOIN _x000d__x000a_pubs.dbo.publishers T5 ON T1.pub_id = T5.pub_id_x000d__x000a_"/>
   </connection>
   <connection id="9" xr16:uid="{B7275D5B-5419-43EF-AC90-462F6DFD7D23}" keepAlive="1" name="Verbindung8" type="5" refreshedVersion="6" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT T2.stor_name AS stor_idLU, T1.ord_num, T1.ord_date, T1.qty, T1.payterms, T7.title AS title_idLU_x000d__x000a_FROM pubs.dbo.sales T1 INNER JOIN _x000d__x000a_pubs.dbo.stores T2 ON T1.stor_id = T2.stor_id INNER JOIN _x000d__x000a_pubs.dbo.titles T7 ON T1.title_id = T7.title_id_x000d__x000a_"/>
+    <dbPr connection="Provider=MSOLEDBSQL.1;Persist Security Info=True;Extended Properties=&quot;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32576;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False;MARS Connection=False;DataTypeCompatibility=0;Trust Server Certificate=False;Application Intent=READWRITE;MultisubnetFailover=False;Use FMTONLY=False" command="SELECT T2.stor_name AS stor_idLU, T1.ord_num, T1.ord_date, T1.qty, T1.payterms, T7.title AS title_idLU_x000d__x000a_FROM pubs.dbo.sales T1 INNER JOIN _x000d__x000a_pubs.dbo.stores T2 ON T1.stor_id = T2.stor_id INNER JOIN _x000d__x000a_pubs.dbo.titles T7 ON T1.title_id = T7.title_id_x000d__x000a_"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="544">
   <si>
     <t xml:space="preserve">SELECT T1.au_id, T1.au_lname, T1.au_fname, T1.phone, T1.address, T1.city, T1.state, T1.zip, T1.contract_x000D_
 FROM pubs.dbo.authors T1 _x000D_
@@ -1782,9 +1782,6 @@
     <t>iuziuz</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Timothy</t>
   </si>
   <si>
@@ -1804,14 +1801,28 @@
   </si>
   <si>
     <t>München</t>
+  </si>
+  <si>
+    <t>notexisting</t>
+  </si>
+  <si>
+    <t>u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1839,12 +1850,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3421,7 +3433,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G25" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle_ExterneDaten_18" displayName="Tabelle_ExterneDaten_18" ref="B1:G26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="6">
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" uniqueName="3" name="au_idLU" queryTableFieldId="2" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" uniqueName="4" name="title_idLU" queryTableFieldId="3" dataDxfId="17"/>
@@ -3723,19 +3735,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
@@ -4254,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>117</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>122</v>
       </c>
@@ -4312,7 +4324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>128</v>
       </c>
@@ -4341,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>133</v>
       </c>
@@ -4370,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>141</v>
       </c>
@@ -4399,7 +4411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>144</v>
       </c>
@@ -4428,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>151</v>
       </c>
@@ -4457,33 +4469,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="J24" s="2" t="b">
+      <c r="J24" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -4918,7 +4931,7 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5580,7 +5593,7 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Tabelle13"/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -6156,12 +6169,34 @@
         <v>PS2106</v>
       </c>
     </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>100</v>
+      </c>
+      <c r="F26" s="2" t="e">
+        <f>IF(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[au_idLU]],au_idLookup,2,FALSE),"")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G26" s="2" t="str">
+        <f>IF(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]]&lt;&gt;"",VLOOKUP(Tabelle_ExterneDaten_18[[#This Row],[title_idLU]],title_idLookup,2,FALSE),"")</f>
+        <v>PS3333</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B25" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>OFFSET(au_idLookup,0,0,,1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C26" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>OFFSET(title_idLookup,0,0,,1)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7959,9 +7994,7 @@
       <c r="C23" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>535</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
         <v>296</v>
       </c>
@@ -8083,9 +8116,7 @@
       <c r="C27" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>535</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>310</v>
       </c>
@@ -8174,7 +8205,7 @@
         <v>317</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>234</v>
@@ -8300,9 +8331,7 @@
       <c r="C34" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>535</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
         <v>331</v>
       </c>
@@ -8393,9 +8422,7 @@
       <c r="C37" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>535</v>
-      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>339</v>
       </c>
@@ -8455,9 +8482,7 @@
       <c r="C39" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>535</v>
-      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
         <v>346</v>
       </c>
@@ -8481,14 +8506,14 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>538</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>193</v>
@@ -8665,7 +8690,7 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>530</v>
@@ -8674,7 +8699,7 @@
         <v>227</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>187</v>
@@ -9157,7 +9182,7 @@
         <v>208</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">

</xml_diff>